<commit_message>
New Python3 / python2 compatible pyMez! Even largely ported wx for frontends. Still some issues in FrontEnds
</commit_message>
<xml_diff>
--- a/Documentation/Examples/jupyter/TableGraph_Files/Test.xlsx
+++ b/Documentation/Examples/jupyter/TableGraph_Files/Test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandersa\PyCharmProjects\Jupyter-Notebooks\TableGraph_Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramData\Anaconda2\Lib\site-packages\pyMez\Documentation\Examples\jupyter\TableGraph_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{367AE64B-FB88-41C1-93A2-29F22BC8BA7D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0DEF803-6F28-4B63-A548-FE51B1D5CEBF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11460" windowHeight="8715"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17460" windowHeight="8715"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>